<commit_message>
menambahkan library stats4 dan lattice
</commit_message>
<xml_diff>
--- a/Skor_PM_1PL.xlsx
+++ b/Skor_PM_1PL.xlsx
@@ -394,7 +394,7 @@
         </is>
       </c>
       <c r="D2">
-        <v>778.3279848830533</v>
+        <v>742.5848606869378</v>
       </c>
     </row>
     <row r="3">
@@ -412,7 +412,7 @@
         </is>
       </c>
       <c r="D3">
-        <v>297.8083388514164</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="4">
@@ -430,7 +430,7 @@
         </is>
       </c>
       <c r="D4">
-        <v>391.9509306202153</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="5">
@@ -466,7 +466,7 @@
         </is>
       </c>
       <c r="D6">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="7">
@@ -484,7 +484,7 @@
         </is>
       </c>
       <c r="D7">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="8">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="D8">
-        <v>391.950930620215</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="9">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="D9">
-        <v>202.1265485002848</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="10">
@@ -538,7 +538,7 @@
         </is>
       </c>
       <c r="D10">
-        <v>202.1265485002847</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="11">
@@ -556,7 +556,7 @@
         </is>
       </c>
       <c r="D11">
-        <v>202.1265485002847</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="12">
@@ -610,7 +610,7 @@
         </is>
       </c>
       <c r="D14">
-        <v>202.1265485002847</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="15">
@@ -646,7 +646,7 @@
         </is>
       </c>
       <c r="D16">
-        <v>297.8083388514165</v>
+        <v>415.8096624832563</v>
       </c>
     </row>
     <row r="17">
@@ -664,7 +664,7 @@
         </is>
       </c>
       <c r="D17">
-        <v>103.6218025752549</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="18">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="D18">
-        <v>202.1265485002848</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="19">
@@ -700,7 +700,7 @@
         </is>
       </c>
       <c r="D19">
-        <v>485.6083947034062</v>
+        <v>539.1303929564187</v>
       </c>
     </row>
     <row r="20">
@@ -718,7 +718,7 @@
         </is>
       </c>
       <c r="D20">
-        <v>778.3279848830533</v>
+        <v>742.5848606869378</v>
       </c>
     </row>
     <row r="21">
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="D21">
-        <v>391.9509306202151</v>
+        <v>479.543115199688</v>
       </c>
     </row>
     <row r="22">
@@ -754,7 +754,7 @@
         </is>
       </c>
       <c r="D22">
-        <v>297.8083388514166</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="23">
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="D23">
-        <v>202.1265485002847</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="24">
@@ -790,7 +790,7 @@
         </is>
       </c>
       <c r="D24">
-        <v>202.1265485002847</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="25">
@@ -808,7 +808,7 @@
         </is>
       </c>
       <c r="D25">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="26">
@@ -826,7 +826,7 @@
         </is>
       </c>
       <c r="D26">
-        <v>677.0733158492224</v>
+        <v>665.0053611702178</v>
       </c>
     </row>
     <row r="27">
@@ -844,7 +844,7 @@
         </is>
       </c>
       <c r="D27">
-        <v>580.0967871035209</v>
+        <v>599.4029459436151</v>
       </c>
     </row>
     <row r="28">
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="D28">
-        <v>677.0733158492224</v>
+        <v>665.0053611702177</v>
       </c>
     </row>
     <row r="29">
@@ -880,7 +880,7 @@
         </is>
       </c>
       <c r="D29">
-        <v>391.950930620215</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="30">
@@ -898,7 +898,7 @@
         </is>
       </c>
       <c r="D30">
-        <v>391.9509306202153</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="31">
@@ -916,7 +916,7 @@
         </is>
       </c>
       <c r="D31">
-        <v>485.6083947034061</v>
+        <v>539.1303929564187</v>
       </c>
     </row>
     <row r="32">
@@ -934,7 +934,7 @@
         </is>
       </c>
       <c r="D32">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="33">
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="D33">
-        <v>778.3279848830533</v>
+        <v>742.5848606869378</v>
       </c>
     </row>
     <row r="34">
@@ -988,7 +988,7 @@
         </is>
       </c>
       <c r="D35">
-        <v>391.950930620215</v>
+        <v>479.5431151996878</v>
       </c>
     </row>
     <row r="36">
@@ -1006,7 +1006,7 @@
         </is>
       </c>
       <c r="D36">
-        <v>485.6083947034062</v>
+        <v>539.1303929564189</v>
       </c>
     </row>
     <row r="37">
@@ -1024,7 +1024,7 @@
         </is>
       </c>
       <c r="D37">
-        <v>297.8083388514165</v>
+        <v>415.8096624832563</v>
       </c>
     </row>
     <row r="38">
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="D38">
-        <v>297.8083388514166</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="39">
@@ -1078,7 +1078,7 @@
         </is>
       </c>
       <c r="D40">
-        <v>580.0967871035209</v>
+        <v>599.4029459436152</v>
       </c>
     </row>
     <row r="41">
@@ -1114,7 +1114,7 @@
         </is>
       </c>
       <c r="D42">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="43">
@@ -1150,7 +1150,7 @@
         </is>
       </c>
       <c r="D44">
-        <v>297.8083388514166</v>
+        <v>415.8096624832563</v>
       </c>
     </row>
     <row r="45">
@@ -1168,7 +1168,7 @@
         </is>
       </c>
       <c r="D45">
-        <v>297.8083388514166</v>
+        <v>415.8096624832563</v>
       </c>
     </row>
     <row r="46">
@@ -1186,7 +1186,7 @@
         </is>
       </c>
       <c r="D46">
-        <v>103.6218025752549</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="47">
@@ -1204,7 +1204,7 @@
         </is>
       </c>
       <c r="D47">
-        <v>297.8083388514167</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="48">
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="D48">
-        <v>103.6218025752549</v>
+        <v>233.0626819566948</v>
       </c>
     </row>
     <row r="49">
@@ -1240,7 +1240,7 @@
         </is>
       </c>
       <c r="D49">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="50">
@@ -1258,7 +1258,7 @@
         </is>
       </c>
       <c r="D50">
-        <v>580.0967871035207</v>
+        <v>599.4029459436151</v>
       </c>
     </row>
     <row r="51">
@@ -1276,7 +1276,7 @@
         </is>
       </c>
       <c r="D51">
-        <v>391.9509306202149</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="52">
@@ -1294,7 +1294,7 @@
         </is>
       </c>
       <c r="D52">
-        <v>677.0733158492224</v>
+        <v>665.0053611702177</v>
       </c>
     </row>
     <row r="53">
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="D53">
-        <v>297.8083388514165</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="54">
@@ -1330,7 +1330,7 @@
         </is>
       </c>
       <c r="D54">
-        <v>580.0967871035208</v>
+        <v>599.4029459436151</v>
       </c>
     </row>
     <row r="55">
@@ -1348,7 +1348,7 @@
         </is>
       </c>
       <c r="D55">
-        <v>202.1265485002847</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="56">
@@ -1366,7 +1366,7 @@
         </is>
       </c>
       <c r="D56">
-        <v>485.6083947034061</v>
+        <v>539.1303929564187</v>
       </c>
     </row>
     <row r="57">
@@ -1384,7 +1384,7 @@
         </is>
       </c>
       <c r="D57">
-        <v>580.0967871035208</v>
+        <v>599.4029459436151</v>
       </c>
     </row>
     <row r="58">
@@ -1402,7 +1402,7 @@
         </is>
       </c>
       <c r="D58">
-        <v>778.3279848830533</v>
+        <v>742.5848606869374</v>
       </c>
     </row>
     <row r="59">
@@ -1420,7 +1420,7 @@
         </is>
       </c>
       <c r="D59">
-        <v>297.8083388514166</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="60">
@@ -1438,7 +1438,7 @@
         </is>
       </c>
       <c r="D60">
-        <v>677.0733158492222</v>
+        <v>665.0053611702178</v>
       </c>
     </row>
     <row r="61">
@@ -1456,7 +1456,7 @@
         </is>
       </c>
       <c r="D61">
-        <v>485.6083947034061</v>
+        <v>539.1303929564189</v>
       </c>
     </row>
     <row r="62">
@@ -1474,7 +1474,7 @@
         </is>
       </c>
       <c r="D62">
-        <v>202.1265485002847</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="63">
@@ -1510,7 +1510,7 @@
         </is>
       </c>
       <c r="D64">
-        <v>580.0967871035208</v>
+        <v>599.4029459436151</v>
       </c>
     </row>
     <row r="65">
@@ -1546,7 +1546,7 @@
         </is>
       </c>
       <c r="D66">
-        <v>202.1265485002849</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="67">
@@ -1564,7 +1564,7 @@
         </is>
       </c>
       <c r="D67">
-        <v>297.8083388514166</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="68">
@@ -1582,7 +1582,7 @@
         </is>
       </c>
       <c r="D68">
-        <v>297.8083388514167</v>
+        <v>415.8096624832563</v>
       </c>
     </row>
     <row r="69">
@@ -1600,7 +1600,7 @@
         </is>
       </c>
       <c r="D69">
-        <v>103.621802575255</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="70">
@@ -1618,7 +1618,7 @@
         </is>
       </c>
       <c r="D70">
-        <v>677.0733158492218</v>
+        <v>665.0053611702178</v>
       </c>
     </row>
     <row r="71">
@@ -1636,7 +1636,7 @@
         </is>
       </c>
       <c r="D71">
-        <v>103.621802575255</v>
+        <v>233.0626819566948</v>
       </c>
     </row>
     <row r="72">
@@ -1654,7 +1654,7 @@
         </is>
       </c>
       <c r="D72">
-        <v>391.9509306202151</v>
+        <v>479.543115199688</v>
       </c>
     </row>
     <row r="73">
@@ -1672,7 +1672,7 @@
         </is>
       </c>
       <c r="D73">
-        <v>202.1265485002847</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="74">
@@ -1690,7 +1690,7 @@
         </is>
       </c>
       <c r="D74">
-        <v>580.0967871035207</v>
+        <v>599.4029459436151</v>
       </c>
     </row>
     <row r="75">
@@ -1708,7 +1708,7 @@
         </is>
       </c>
       <c r="D75">
-        <v>677.0733158492224</v>
+        <v>665.0053611702177</v>
       </c>
     </row>
     <row r="76">
@@ -1726,7 +1726,7 @@
         </is>
       </c>
       <c r="D76">
-        <v>297.8083388514167</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="77">
@@ -1744,7 +1744,7 @@
         </is>
       </c>
       <c r="D77">
-        <v>297.8083388514165</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="78">
@@ -1798,7 +1798,7 @@
         </is>
       </c>
       <c r="D80">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="81">
@@ -1816,7 +1816,7 @@
         </is>
       </c>
       <c r="D81">
-        <v>485.6083947034061</v>
+        <v>539.1303929564189</v>
       </c>
     </row>
     <row r="82">
@@ -1834,7 +1834,7 @@
         </is>
       </c>
       <c r="D82">
-        <v>202.1265485002847</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="83">
@@ -1852,7 +1852,7 @@
         </is>
       </c>
       <c r="D83">
-        <v>202.1265485002849</v>
+        <v>340.1864117793779</v>
       </c>
     </row>
     <row r="84">
@@ -1888,7 +1888,7 @@
         </is>
       </c>
       <c r="D85">
-        <v>103.6218025752551</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="86">
@@ -1906,7 +1906,7 @@
         </is>
       </c>
       <c r="D86">
-        <v>485.6083947034061</v>
+        <v>539.1303929564187</v>
       </c>
     </row>
     <row r="87">
@@ -1924,7 +1924,7 @@
         </is>
       </c>
       <c r="D87">
-        <v>885.5095393821985</v>
+        <v>846.0391805322012</v>
       </c>
     </row>
     <row r="88">
@@ -1942,7 +1942,7 @@
         </is>
       </c>
       <c r="D88">
-        <v>297.8083388514166</v>
+        <v>415.8096624832563</v>
       </c>
     </row>
     <row r="89">
@@ -1960,7 +1960,7 @@
         </is>
       </c>
       <c r="D89">
-        <v>580.0967871035208</v>
+        <v>599.4029459436151</v>
       </c>
     </row>
     <row r="90">
@@ -1978,7 +1978,7 @@
         </is>
       </c>
       <c r="D90">
-        <v>391.9509306202151</v>
+        <v>479.543115199688</v>
       </c>
     </row>
     <row r="91">
@@ -1996,7 +1996,7 @@
         </is>
       </c>
       <c r="D91">
-        <v>202.1265485002849</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="92">
@@ -2014,7 +2014,7 @@
         </is>
       </c>
       <c r="D92">
-        <v>485.6083947034061</v>
+        <v>539.1303929564189</v>
       </c>
     </row>
     <row r="93">
@@ -2032,7 +2032,7 @@
         </is>
       </c>
       <c r="D93">
-        <v>297.8083388514167</v>
+        <v>415.8096624832563</v>
       </c>
     </row>
     <row r="94">
@@ -2068,7 +2068,7 @@
         </is>
       </c>
       <c r="D95">
-        <v>391.9509306202152</v>
+        <v>479.5431151996878</v>
       </c>
     </row>
     <row r="96">
@@ -2086,7 +2086,7 @@
         </is>
       </c>
       <c r="D96">
-        <v>391.9509306202152</v>
+        <v>479.5431151996878</v>
       </c>
     </row>
     <row r="97">
@@ -2104,7 +2104,7 @@
         </is>
       </c>
       <c r="D97">
-        <v>580.096787103521</v>
+        <v>599.4029459436152</v>
       </c>
     </row>
     <row r="98">
@@ -2140,7 +2140,7 @@
         </is>
       </c>
       <c r="D99">
-        <v>485.6083947034062</v>
+        <v>539.1303929564191</v>
       </c>
     </row>
     <row r="100">
@@ -2158,7 +2158,7 @@
         </is>
       </c>
       <c r="D100">
-        <v>391.9509306202152</v>
+        <v>479.543115199688</v>
       </c>
     </row>
     <row r="101">
@@ -2194,7 +2194,7 @@
         </is>
       </c>
       <c r="D102">
-        <v>297.8083388514165</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="103">
@@ -2212,7 +2212,7 @@
         </is>
       </c>
       <c r="D103">
-        <v>391.9509306202149</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="104">
@@ -2230,7 +2230,7 @@
         </is>
       </c>
       <c r="D104">
-        <v>778.3279848830532</v>
+        <v>742.5848606869374</v>
       </c>
     </row>
     <row r="105">
@@ -2248,7 +2248,7 @@
         </is>
       </c>
       <c r="D105">
-        <v>297.8083388514166</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="106">
@@ -2284,7 +2284,7 @@
         </is>
       </c>
       <c r="D107">
-        <v>103.621802575255</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="108">
@@ -2302,7 +2302,7 @@
         </is>
       </c>
       <c r="D108">
-        <v>103.621802575255</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="109">
@@ -2320,7 +2320,7 @@
         </is>
       </c>
       <c r="D109">
-        <v>778.3279848830533</v>
+        <v>742.5848606869376</v>
       </c>
     </row>
     <row r="110">
@@ -2338,7 +2338,7 @@
         </is>
       </c>
       <c r="D110">
-        <v>103.6218025752549</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="111">
@@ -2374,7 +2374,7 @@
         </is>
       </c>
       <c r="D112">
-        <v>485.6083947034062</v>
+        <v>539.1303929564189</v>
       </c>
     </row>
     <row r="113">
@@ -2392,7 +2392,7 @@
         </is>
       </c>
       <c r="D113">
-        <v>778.3279848830533</v>
+        <v>742.5848606869376</v>
       </c>
     </row>
     <row r="114">
@@ -2410,7 +2410,7 @@
         </is>
       </c>
       <c r="D114">
-        <v>297.8083388514166</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="115">
@@ -2428,7 +2428,7 @@
         </is>
       </c>
       <c r="D115">
-        <v>202.1265485002847</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="116">
@@ -2446,7 +2446,7 @@
         </is>
       </c>
       <c r="D116">
-        <v>202.1265485002847</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="117">
@@ -2464,7 +2464,7 @@
         </is>
       </c>
       <c r="D117">
-        <v>202.1265485002849</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="118">
@@ -2536,7 +2536,7 @@
         </is>
       </c>
       <c r="D121">
-        <v>103.621802575255</v>
+        <v>233.0626819566948</v>
       </c>
     </row>
     <row r="122">
@@ -2554,7 +2554,7 @@
         </is>
       </c>
       <c r="D122">
-        <v>391.9509306202151</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="123">
@@ -2590,7 +2590,7 @@
         </is>
       </c>
       <c r="D124">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="125">
@@ -2608,7 +2608,7 @@
         </is>
       </c>
       <c r="D125">
-        <v>202.1265485002848</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="126">
@@ -2626,7 +2626,7 @@
         </is>
       </c>
       <c r="D126">
-        <v>391.9509306202152</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="127">
@@ -2644,7 +2644,7 @@
         </is>
       </c>
       <c r="D127">
-        <v>103.621802575255</v>
+        <v>233.0626819566948</v>
       </c>
     </row>
     <row r="128">
@@ -2680,7 +2680,7 @@
         </is>
       </c>
       <c r="D129">
-        <v>297.8083388514166</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="130">
@@ -2698,7 +2698,7 @@
         </is>
       </c>
       <c r="D130">
-        <v>778.3279848830533</v>
+        <v>742.5848606869375</v>
       </c>
     </row>
     <row r="131">
@@ -2716,7 +2716,7 @@
         </is>
       </c>
       <c r="D131">
-        <v>202.1265485002847</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="132">
@@ -2734,7 +2734,7 @@
         </is>
       </c>
       <c r="D132">
-        <v>391.950930620215</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="133">
@@ -2752,7 +2752,7 @@
         </is>
       </c>
       <c r="D133">
-        <v>580.0967871035214</v>
+        <v>599.4029459436154</v>
       </c>
     </row>
     <row r="134">
@@ -2806,7 +2806,7 @@
         </is>
       </c>
       <c r="D136">
-        <v>297.8083388514167</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="137">
@@ -2842,7 +2842,7 @@
         </is>
       </c>
       <c r="D138">
-        <v>677.073315849222</v>
+        <v>665.0053611702178</v>
       </c>
     </row>
     <row r="139">
@@ -2860,7 +2860,7 @@
         </is>
       </c>
       <c r="D139">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="140">
@@ -2878,7 +2878,7 @@
         </is>
       </c>
       <c r="D140">
-        <v>485.6083947034064</v>
+        <v>539.1303929564191</v>
       </c>
     </row>
     <row r="141">
@@ -2896,7 +2896,7 @@
         </is>
       </c>
       <c r="D141">
-        <v>677.0733158492224</v>
+        <v>665.0053611702175</v>
       </c>
     </row>
     <row r="142">
@@ -2914,7 +2914,7 @@
         </is>
       </c>
       <c r="D142">
-        <v>580.0967871035207</v>
+        <v>599.4029459436154</v>
       </c>
     </row>
     <row r="143">
@@ -2932,7 +2932,7 @@
         </is>
       </c>
       <c r="D143">
-        <v>580.096787103521</v>
+        <v>599.4029459436151</v>
       </c>
     </row>
     <row r="144">
@@ -2950,7 +2950,7 @@
         </is>
       </c>
       <c r="D144">
-        <v>202.1265485002847</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="145">
@@ -2968,7 +2968,7 @@
         </is>
       </c>
       <c r="D145">
-        <v>103.6218025752549</v>
+        <v>233.0626819566948</v>
       </c>
     </row>
     <row r="146">
@@ -2986,7 +2986,7 @@
         </is>
       </c>
       <c r="D146">
-        <v>297.8083388514165</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="147">
@@ -3004,7 +3004,7 @@
         </is>
       </c>
       <c r="D147">
-        <v>103.621802575255</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="148">
@@ -3022,7 +3022,7 @@
         </is>
       </c>
       <c r="D148">
-        <v>391.950930620215</v>
+        <v>479.5431151996878</v>
       </c>
     </row>
     <row r="149">
@@ -3040,7 +3040,7 @@
         </is>
       </c>
       <c r="D149">
-        <v>580.0967871035207</v>
+        <v>599.4029459436154</v>
       </c>
     </row>
     <row r="150">
@@ -3058,7 +3058,7 @@
         </is>
       </c>
       <c r="D150">
-        <v>297.8083388514164</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="151">
@@ -3076,7 +3076,7 @@
         </is>
       </c>
       <c r="D151">
-        <v>485.6083947034062</v>
+        <v>539.1303929564189</v>
       </c>
     </row>
     <row r="152">
@@ -3094,7 +3094,7 @@
         </is>
       </c>
       <c r="D152">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="153">
@@ -3112,7 +3112,7 @@
         </is>
       </c>
       <c r="D153">
-        <v>391.9509306202152</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="154">
@@ -3148,7 +3148,7 @@
         </is>
       </c>
       <c r="D155">
-        <v>103.621802575255</v>
+        <v>233.0626819566948</v>
       </c>
     </row>
     <row r="156">
@@ -3166,7 +3166,7 @@
         </is>
       </c>
       <c r="D156">
-        <v>580.096787103521</v>
+        <v>599.4029459436151</v>
       </c>
     </row>
     <row r="157">
@@ -3184,7 +3184,7 @@
         </is>
       </c>
       <c r="D157">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="158">
@@ -3202,7 +3202,7 @@
         </is>
       </c>
       <c r="D158">
-        <v>297.8083388514166</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="159">
@@ -3220,7 +3220,7 @@
         </is>
       </c>
       <c r="D159">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="160">
@@ -3238,7 +3238,7 @@
         </is>
       </c>
       <c r="D160">
-        <v>297.8083388514166</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="161">
@@ -3256,7 +3256,7 @@
         </is>
       </c>
       <c r="D161">
-        <v>103.6218025752551</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="162">
@@ -3274,7 +3274,7 @@
         </is>
       </c>
       <c r="D162">
-        <v>580.0967871035213</v>
+        <v>599.4029459436151</v>
       </c>
     </row>
     <row r="163">
@@ -3292,7 +3292,7 @@
         </is>
       </c>
       <c r="D163">
-        <v>580.0967871035207</v>
+        <v>599.4029459436154</v>
       </c>
     </row>
     <row r="164">
@@ -3328,7 +3328,7 @@
         </is>
       </c>
       <c r="D165">
-        <v>297.8083388514167</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="166">
@@ -3346,7 +3346,7 @@
         </is>
       </c>
       <c r="D166">
-        <v>297.8083388514167</v>
+        <v>415.8096624832563</v>
       </c>
     </row>
     <row r="167">
@@ -3382,7 +3382,7 @@
         </is>
       </c>
       <c r="D168">
-        <v>202.1265485002847</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="169">
@@ -3400,7 +3400,7 @@
         </is>
       </c>
       <c r="D169">
-        <v>202.1265485002849</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="170">
@@ -3418,7 +3418,7 @@
         </is>
       </c>
       <c r="D170">
-        <v>580.096787103521</v>
+        <v>599.4029459436152</v>
       </c>
     </row>
     <row r="171">
@@ -3436,7 +3436,7 @@
         </is>
       </c>
       <c r="D171">
-        <v>391.950930620215</v>
+        <v>479.5431151996878</v>
       </c>
     </row>
     <row r="172">
@@ -3454,7 +3454,7 @@
         </is>
       </c>
       <c r="D172">
-        <v>778.3279848830533</v>
+        <v>742.5848606869374</v>
       </c>
     </row>
     <row r="173">
@@ -3472,7 +3472,7 @@
         </is>
       </c>
       <c r="D173">
-        <v>391.9509306202149</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="174">
@@ -3508,7 +3508,7 @@
         </is>
       </c>
       <c r="D175">
-        <v>202.1265485002849</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="176">
@@ -3562,7 +3562,7 @@
         </is>
       </c>
       <c r="D178">
-        <v>580.0967871035208</v>
+        <v>599.4029459436151</v>
       </c>
     </row>
     <row r="179">
@@ -3580,7 +3580,7 @@
         </is>
       </c>
       <c r="D179">
-        <v>202.126548500285</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="180">
@@ -3598,7 +3598,7 @@
         </is>
       </c>
       <c r="D180">
-        <v>202.1265485002849</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="181">
@@ -3634,7 +3634,7 @@
         </is>
       </c>
       <c r="D182">
-        <v>297.8083388514167</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="183">
@@ -3652,7 +3652,7 @@
         </is>
       </c>
       <c r="D183">
-        <v>297.8083388514166</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="184">
@@ -3688,7 +3688,7 @@
         </is>
       </c>
       <c r="D185">
-        <v>391.9509306202151</v>
+        <v>479.543115199688</v>
       </c>
     </row>
     <row r="186">
@@ -3706,7 +3706,7 @@
         </is>
       </c>
       <c r="D186">
-        <v>391.9509306202152</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="187">
@@ -3724,7 +3724,7 @@
         </is>
       </c>
       <c r="D187">
-        <v>202.1265485002849</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="188">
@@ -3778,7 +3778,7 @@
         </is>
       </c>
       <c r="D190">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="191">
@@ -3796,7 +3796,7 @@
         </is>
       </c>
       <c r="D191">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="192">
@@ -3814,7 +3814,7 @@
         </is>
       </c>
       <c r="D192">
-        <v>297.8083388514165</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="193">
@@ -3850,7 +3850,7 @@
         </is>
       </c>
       <c r="D194">
-        <v>202.1265485002847</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="195">
@@ -3868,7 +3868,7 @@
         </is>
       </c>
       <c r="D195">
-        <v>778.3279848830532</v>
+        <v>742.5848606869378</v>
       </c>
     </row>
     <row r="196">
@@ -3886,7 +3886,7 @@
         </is>
       </c>
       <c r="D196">
-        <v>202.1265485002849</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="197">
@@ -3904,7 +3904,7 @@
         </is>
       </c>
       <c r="D197">
-        <v>103.6218025752549</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="198">
@@ -3922,7 +3922,7 @@
         </is>
       </c>
       <c r="D198">
-        <v>202.1265485002848</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="199">
@@ -3940,7 +3940,7 @@
         </is>
       </c>
       <c r="D199">
-        <v>391.9509306202148</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="200">
@@ -3958,7 +3958,7 @@
         </is>
       </c>
       <c r="D200">
-        <v>778.3279848830535</v>
+        <v>742.5848606869376</v>
       </c>
     </row>
     <row r="201">
@@ -3976,7 +3976,7 @@
         </is>
       </c>
       <c r="D201">
-        <v>391.9509306202151</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="202">
@@ -3994,7 +3994,7 @@
         </is>
       </c>
       <c r="D202">
-        <v>103.6218025752549</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="203">
@@ -4012,7 +4012,7 @@
         </is>
       </c>
       <c r="D203">
-        <v>485.6083947034061</v>
+        <v>539.1303929564189</v>
       </c>
     </row>
     <row r="204">
@@ -4048,7 +4048,7 @@
         </is>
       </c>
       <c r="D205">
-        <v>485.6083947034064</v>
+        <v>539.1303929564189</v>
       </c>
     </row>
     <row r="206">
@@ -4066,7 +4066,7 @@
         </is>
       </c>
       <c r="D206">
-        <v>297.8083388514166</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="207">
@@ -4084,7 +4084,7 @@
         </is>
       </c>
       <c r="D207">
-        <v>391.950930620215</v>
+        <v>479.543115199688</v>
       </c>
     </row>
     <row r="208">
@@ -4102,7 +4102,7 @@
         </is>
       </c>
       <c r="D208">
-        <v>297.8083388514165</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="209">
@@ -4120,7 +4120,7 @@
         </is>
       </c>
       <c r="D209">
-        <v>485.6083947034061</v>
+        <v>539.130392956419</v>
       </c>
     </row>
     <row r="210">
@@ -4138,7 +4138,7 @@
         </is>
       </c>
       <c r="D210">
-        <v>778.3279848830533</v>
+        <v>742.5848606869378</v>
       </c>
     </row>
     <row r="211">
@@ -4156,7 +4156,7 @@
         </is>
       </c>
       <c r="D211">
-        <v>202.1265485002849</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="212">
@@ -4174,7 +4174,7 @@
         </is>
       </c>
       <c r="D212">
-        <v>103.6218025752551</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="213">
@@ -4210,7 +4210,7 @@
         </is>
       </c>
       <c r="D214">
-        <v>677.0733158492224</v>
+        <v>665.0053611702178</v>
       </c>
     </row>
     <row r="215">
@@ -4228,7 +4228,7 @@
         </is>
       </c>
       <c r="D215">
-        <v>297.8083388514164</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="216">
@@ -4264,7 +4264,7 @@
         </is>
       </c>
       <c r="D217">
-        <v>580.0967871035213</v>
+        <v>599.4029459436151</v>
       </c>
     </row>
     <row r="218">
@@ -4282,7 +4282,7 @@
         </is>
       </c>
       <c r="D218">
-        <v>103.6218025752549</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="219">
@@ -4300,7 +4300,7 @@
         </is>
       </c>
       <c r="D219">
-        <v>202.1265485002849</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="220">
@@ -4318,7 +4318,7 @@
         </is>
       </c>
       <c r="D220">
-        <v>103.621802575255</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="221">
@@ -4354,7 +4354,7 @@
         </is>
       </c>
       <c r="D222">
-        <v>202.1265485002849</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="223">
@@ -4372,7 +4372,7 @@
         </is>
       </c>
       <c r="D223">
-        <v>297.8083388514166</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="224">
@@ -4390,7 +4390,7 @@
         </is>
       </c>
       <c r="D224">
-        <v>778.3279848830533</v>
+        <v>742.5848606869374</v>
       </c>
     </row>
     <row r="225">
@@ -4408,7 +4408,7 @@
         </is>
       </c>
       <c r="D225">
-        <v>778.3279848830538</v>
+        <v>742.5848606869375</v>
       </c>
     </row>
     <row r="226">
@@ -4426,7 +4426,7 @@
         </is>
       </c>
       <c r="D226">
-        <v>391.9509306202149</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="227">
@@ -4444,7 +4444,7 @@
         </is>
       </c>
       <c r="D227">
-        <v>485.6083947034061</v>
+        <v>539.1303929564189</v>
       </c>
     </row>
     <row r="228">
@@ -4498,7 +4498,7 @@
         </is>
       </c>
       <c r="D230">
-        <v>297.8083388514166</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="231">
@@ -4534,7 +4534,7 @@
         </is>
       </c>
       <c r="D232">
-        <v>297.8083388514166</v>
+        <v>415.8096624832563</v>
       </c>
     </row>
     <row r="233">
@@ -4552,7 +4552,7 @@
         </is>
       </c>
       <c r="D233">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="234">
@@ -4570,7 +4570,7 @@
         </is>
       </c>
       <c r="D234">
-        <v>202.1265485002849</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="235">
@@ -4624,7 +4624,7 @@
         </is>
       </c>
       <c r="D237">
-        <v>391.9509306202151</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="238">
@@ -4642,7 +4642,7 @@
         </is>
       </c>
       <c r="D238">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="239">
@@ -4660,7 +4660,7 @@
         </is>
       </c>
       <c r="D239">
-        <v>297.8083388514165</v>
+        <v>415.8096624832563</v>
       </c>
     </row>
     <row r="240">
@@ -4678,7 +4678,7 @@
         </is>
       </c>
       <c r="D240">
-        <v>103.6218025752549</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="241">
@@ -4696,7 +4696,7 @@
         </is>
       </c>
       <c r="D241">
-        <v>580.096787103521</v>
+        <v>599.4029459436152</v>
       </c>
     </row>
     <row r="242">
@@ -4714,7 +4714,7 @@
         </is>
       </c>
       <c r="D242">
-        <v>391.9509306202152</v>
+        <v>479.5431151996881</v>
       </c>
     </row>
     <row r="243">
@@ -4750,7 +4750,7 @@
         </is>
       </c>
       <c r="D244">
-        <v>778.3279848830533</v>
+        <v>742.5848606869374</v>
       </c>
     </row>
     <row r="245">
@@ -4768,7 +4768,7 @@
         </is>
       </c>
       <c r="D245">
-        <v>778.3279848830527</v>
+        <v>742.5848606869376</v>
       </c>
     </row>
     <row r="246">
@@ -4786,7 +4786,7 @@
         </is>
       </c>
       <c r="D246">
-        <v>202.1265485002849</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="247">
@@ -4804,7 +4804,7 @@
         </is>
       </c>
       <c r="D247">
-        <v>202.1265485002847</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="248">
@@ -4840,7 +4840,7 @@
         </is>
       </c>
       <c r="D249">
-        <v>297.8083388514166</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="250">
@@ -4858,7 +4858,7 @@
         </is>
       </c>
       <c r="D250">
-        <v>297.8083388514167</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="251">
@@ -4876,7 +4876,7 @@
         </is>
       </c>
       <c r="D251">
-        <v>202.1265485002849</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="252">
@@ -4894,7 +4894,7 @@
         </is>
       </c>
       <c r="D252">
-        <v>297.8083388514168</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="253">
@@ -4912,7 +4912,7 @@
         </is>
       </c>
       <c r="D253">
-        <v>103.621802575255</v>
+        <v>233.0626819566948</v>
       </c>
     </row>
     <row r="254">
@@ -4930,7 +4930,7 @@
         </is>
       </c>
       <c r="D254">
-        <v>580.0967871035206</v>
+        <v>599.4029459436154</v>
       </c>
     </row>
     <row r="255">
@@ -4948,7 +4948,7 @@
         </is>
       </c>
       <c r="D255">
-        <v>391.950930620215</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="256">
@@ -4966,7 +4966,7 @@
         </is>
       </c>
       <c r="D256">
-        <v>677.0733158492226</v>
+        <v>665.0053611702178</v>
       </c>
     </row>
     <row r="257">
@@ -4984,7 +4984,7 @@
         </is>
       </c>
       <c r="D257">
-        <v>391.9509306202149</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="258">
@@ -5020,7 +5020,7 @@
         </is>
       </c>
       <c r="D259">
-        <v>202.1265485002849</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="260">
@@ -5038,7 +5038,7 @@
         </is>
       </c>
       <c r="D260">
-        <v>778.3279848830535</v>
+        <v>742.5848606869376</v>
       </c>
     </row>
     <row r="261">
@@ -5056,7 +5056,7 @@
         </is>
       </c>
       <c r="D261">
-        <v>677.0733158492226</v>
+        <v>665.0053611702178</v>
       </c>
     </row>
     <row r="262">
@@ -5074,7 +5074,7 @@
         </is>
       </c>
       <c r="D262">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="263">
@@ -5092,7 +5092,7 @@
         </is>
       </c>
       <c r="D263">
-        <v>580.0967871035208</v>
+        <v>599.4029459436151</v>
       </c>
     </row>
     <row r="264">
@@ -5128,7 +5128,7 @@
         </is>
       </c>
       <c r="D265">
-        <v>103.621802575255</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="266">
@@ -5146,7 +5146,7 @@
         </is>
       </c>
       <c r="D266">
-        <v>297.8083388514166</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="267">
@@ -5164,7 +5164,7 @@
         </is>
       </c>
       <c r="D267">
-        <v>391.950930620215</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="268">
@@ -5182,7 +5182,7 @@
         </is>
       </c>
       <c r="D268">
-        <v>485.6083947034062</v>
+        <v>539.1303929564187</v>
       </c>
     </row>
     <row r="269">
@@ -5200,7 +5200,7 @@
         </is>
       </c>
       <c r="D269">
-        <v>202.1265485002848</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="270">
@@ -5218,7 +5218,7 @@
         </is>
       </c>
       <c r="D270">
-        <v>103.621802575255</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="271">
@@ -5236,7 +5236,7 @@
         </is>
       </c>
       <c r="D271">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="272">
@@ -5254,7 +5254,7 @@
         </is>
       </c>
       <c r="D272">
-        <v>202.1265485002848</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="273">
@@ -5272,7 +5272,7 @@
         </is>
       </c>
       <c r="D273">
-        <v>485.6083947034062</v>
+        <v>539.1303929564189</v>
       </c>
     </row>
     <row r="274">
@@ -5290,7 +5290,7 @@
         </is>
       </c>
       <c r="D274">
-        <v>778.3279848830535</v>
+        <v>742.5848606869376</v>
       </c>
     </row>
     <row r="275">
@@ -5326,7 +5326,7 @@
         </is>
       </c>
       <c r="D276">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="277">
@@ -5344,7 +5344,7 @@
         </is>
       </c>
       <c r="D277">
-        <v>297.8083388514167</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="278">
@@ -5362,7 +5362,7 @@
         </is>
       </c>
       <c r="D278">
-        <v>202.1265485002849</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="279">
@@ -5380,7 +5380,7 @@
         </is>
       </c>
       <c r="D279">
-        <v>580.0967871035208</v>
+        <v>599.4029459436151</v>
       </c>
     </row>
     <row r="280">
@@ -5398,7 +5398,7 @@
         </is>
       </c>
       <c r="D280">
-        <v>297.8083388514166</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="281">
@@ -5434,7 +5434,7 @@
         </is>
       </c>
       <c r="D282">
-        <v>297.8083388514167</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="283">
@@ -5452,7 +5452,7 @@
         </is>
       </c>
       <c r="D283">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="284">
@@ -5470,7 +5470,7 @@
         </is>
       </c>
       <c r="D284">
-        <v>297.8083388514166</v>
+        <v>415.8096624832563</v>
       </c>
     </row>
     <row r="285">
@@ -5488,7 +5488,7 @@
         </is>
       </c>
       <c r="D285">
-        <v>391.9509306202151</v>
+        <v>479.5431151996878</v>
       </c>
     </row>
     <row r="286">
@@ -5506,7 +5506,7 @@
         </is>
       </c>
       <c r="D286">
-        <v>580.0967871035207</v>
+        <v>599.4029459436154</v>
       </c>
     </row>
     <row r="287">
@@ -5524,7 +5524,7 @@
         </is>
       </c>
       <c r="D287">
-        <v>580.0967871035207</v>
+        <v>599.4029459436151</v>
       </c>
     </row>
     <row r="288">
@@ -5560,7 +5560,7 @@
         </is>
       </c>
       <c r="D289">
-        <v>580.0967871035209</v>
+        <v>599.4029459436154</v>
       </c>
     </row>
     <row r="290">
@@ -5578,7 +5578,7 @@
         </is>
       </c>
       <c r="D290">
-        <v>297.8083388514167</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="291">
@@ -5596,7 +5596,7 @@
         </is>
       </c>
       <c r="D291">
-        <v>391.9509306202152</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="292">
@@ -5614,7 +5614,7 @@
         </is>
       </c>
       <c r="D292">
-        <v>391.9509306202149</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="293">
@@ -5632,7 +5632,7 @@
         </is>
       </c>
       <c r="D293">
-        <v>391.9509306202151</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="294">
@@ -5650,7 +5650,7 @@
         </is>
       </c>
       <c r="D294">
-        <v>885.5095393821985</v>
+        <v>846.0391805322005</v>
       </c>
     </row>
     <row r="295">
@@ -5668,7 +5668,7 @@
         </is>
       </c>
       <c r="D295">
-        <v>202.1265485002849</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="296">
@@ -5686,7 +5686,7 @@
         </is>
       </c>
       <c r="D296">
-        <v>485.6083947034062</v>
+        <v>539.1303929564191</v>
       </c>
     </row>
     <row r="297">
@@ -5740,7 +5740,7 @@
         </is>
       </c>
       <c r="D299">
-        <v>297.8083388514166</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="300">
@@ -5758,7 +5758,7 @@
         </is>
       </c>
       <c r="D300">
-        <v>677.0733158492222</v>
+        <v>665.0053611702178</v>
       </c>
     </row>
     <row r="301">
@@ -5776,7 +5776,7 @@
         </is>
       </c>
       <c r="D301">
-        <v>485.6083947034062</v>
+        <v>539.130392956419</v>
       </c>
     </row>
     <row r="302">
@@ -5794,7 +5794,7 @@
         </is>
       </c>
       <c r="D302">
-        <v>677.0733158492221</v>
+        <v>665.0053611702177</v>
       </c>
     </row>
     <row r="303">
@@ -5812,7 +5812,7 @@
         </is>
       </c>
       <c r="D303">
-        <v>297.8083388514167</v>
+        <v>415.8096624832563</v>
       </c>
     </row>
     <row r="304">
@@ -5848,7 +5848,7 @@
         </is>
       </c>
       <c r="D305">
-        <v>103.6218025752549</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="306">
@@ -5884,7 +5884,7 @@
         </is>
       </c>
       <c r="D307">
-        <v>103.6218025752549</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="308">
@@ -5902,7 +5902,7 @@
         </is>
       </c>
       <c r="D308">
-        <v>103.6218025752551</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="309">
@@ -5920,7 +5920,7 @@
         </is>
       </c>
       <c r="D309">
-        <v>391.950930620215</v>
+        <v>479.5431151996878</v>
       </c>
     </row>
     <row r="310">
@@ -5938,7 +5938,7 @@
         </is>
       </c>
       <c r="D310">
-        <v>485.6083947034061</v>
+        <v>539.1303929564187</v>
       </c>
     </row>
     <row r="311">
@@ -5956,7 +5956,7 @@
         </is>
       </c>
       <c r="D311">
-        <v>202.1265485002848</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="312">
@@ -5974,7 +5974,7 @@
         </is>
       </c>
       <c r="D312">
-        <v>580.0967871035209</v>
+        <v>599.4029459436151</v>
       </c>
     </row>
     <row r="313">
@@ -5992,7 +5992,7 @@
         </is>
       </c>
       <c r="D313">
-        <v>297.8083388514167</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="314">
@@ -6010,7 +6010,7 @@
         </is>
       </c>
       <c r="D314">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="315">
@@ -6028,7 +6028,7 @@
         </is>
       </c>
       <c r="D315">
-        <v>202.1265485002847</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="316">
@@ -6046,7 +6046,7 @@
         </is>
       </c>
       <c r="D316">
-        <v>778.3279848830532</v>
+        <v>742.5848606869376</v>
       </c>
     </row>
     <row r="317">
@@ -6082,7 +6082,7 @@
         </is>
       </c>
       <c r="D318">
-        <v>485.6083947034061</v>
+        <v>539.1303929564189</v>
       </c>
     </row>
     <row r="319">
@@ -6100,7 +6100,7 @@
         </is>
       </c>
       <c r="D319">
-        <v>391.9509306202152</v>
+        <v>479.5431151996878</v>
       </c>
     </row>
     <row r="320">
@@ -6118,7 +6118,7 @@
         </is>
       </c>
       <c r="D320">
-        <v>580.0967871035208</v>
+        <v>599.4029459436154</v>
       </c>
     </row>
     <row r="321">
@@ -6136,7 +6136,7 @@
         </is>
       </c>
       <c r="D321">
-        <v>202.126548500285</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="322">
@@ -6154,7 +6154,7 @@
         </is>
       </c>
       <c r="D322">
-        <v>103.6218025752552</v>
+        <v>233.062681956695</v>
       </c>
     </row>
     <row r="323">
@@ -6172,7 +6172,7 @@
         </is>
       </c>
       <c r="D323">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="324">
@@ -6190,7 +6190,7 @@
         </is>
       </c>
       <c r="D324">
-        <v>580.0967871035207</v>
+        <v>599.4029459436154</v>
       </c>
     </row>
     <row r="325">
@@ -6208,7 +6208,7 @@
         </is>
       </c>
       <c r="D325">
-        <v>103.621802575255</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="326">
@@ -6226,7 +6226,7 @@
         </is>
       </c>
       <c r="D326">
-        <v>677.0733158492222</v>
+        <v>665.0053611702177</v>
       </c>
     </row>
     <row r="327">
@@ -6244,7 +6244,7 @@
         </is>
       </c>
       <c r="D327">
-        <v>202.1265485002849</v>
+        <v>340.1864117793779</v>
       </c>
     </row>
     <row r="328">
@@ -6262,7 +6262,7 @@
         </is>
       </c>
       <c r="D328">
-        <v>202.1265485002847</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="329">
@@ -6280,7 +6280,7 @@
         </is>
       </c>
       <c r="D329">
-        <v>677.0733158492221</v>
+        <v>665.0053611702178</v>
       </c>
     </row>
     <row r="330">
@@ -6298,7 +6298,7 @@
         </is>
       </c>
       <c r="D330">
-        <v>580.0967871035207</v>
+        <v>599.4029459436151</v>
       </c>
     </row>
     <row r="331">
@@ -6316,7 +6316,7 @@
         </is>
       </c>
       <c r="D331">
-        <v>485.6083947034062</v>
+        <v>539.130392956419</v>
       </c>
     </row>
     <row r="332">
@@ -6334,7 +6334,7 @@
         </is>
       </c>
       <c r="D332">
-        <v>202.1265485002848</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="333">
@@ -6352,7 +6352,7 @@
         </is>
       </c>
       <c r="D333">
-        <v>202.1265485002847</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="334">
@@ -6370,7 +6370,7 @@
         </is>
       </c>
       <c r="D334">
-        <v>297.8083388514167</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="335">
@@ -6460,7 +6460,7 @@
         </is>
       </c>
       <c r="D339">
-        <v>103.6218025752549</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="340">
@@ -6478,7 +6478,7 @@
         </is>
       </c>
       <c r="D340">
-        <v>580.096787103521</v>
+        <v>599.4029459436154</v>
       </c>
     </row>
     <row r="341">
@@ -6514,7 +6514,7 @@
         </is>
       </c>
       <c r="D342">
-        <v>297.8083388514165</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="343">
@@ -6532,7 +6532,7 @@
         </is>
       </c>
       <c r="D343">
-        <v>778.3279848830532</v>
+        <v>742.5848606869374</v>
       </c>
     </row>
     <row r="344">
@@ -6586,7 +6586,7 @@
         </is>
       </c>
       <c r="D346">
-        <v>202.1265485002849</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="347">
@@ -6604,7 +6604,7 @@
         </is>
       </c>
       <c r="D347">
-        <v>391.9509306202152</v>
+        <v>479.5431151996877</v>
       </c>
     </row>
     <row r="348">
@@ -6622,7 +6622,7 @@
         </is>
       </c>
       <c r="D348">
-        <v>580.0967871035208</v>
+        <v>599.4029459436151</v>
       </c>
     </row>
     <row r="349">
@@ -6640,7 +6640,7 @@
         </is>
       </c>
       <c r="D349">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="350">
@@ -6658,7 +6658,7 @@
         </is>
       </c>
       <c r="D350">
-        <v>391.9509306202152</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="351">
@@ -6676,7 +6676,7 @@
         </is>
       </c>
       <c r="D351">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="352">
@@ -6694,7 +6694,7 @@
         </is>
       </c>
       <c r="D352">
-        <v>103.621802575255</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="353">
@@ -6712,7 +6712,7 @@
         </is>
       </c>
       <c r="D353">
-        <v>297.8083388514165</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="354">
@@ -6730,7 +6730,7 @@
         </is>
       </c>
       <c r="D354">
-        <v>202.1265485002849</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="355">
@@ -6748,7 +6748,7 @@
         </is>
       </c>
       <c r="D355">
-        <v>202.1265485002849</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="356">
@@ -6766,7 +6766,7 @@
         </is>
       </c>
       <c r="D356">
-        <v>202.1265485002849</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="357">
@@ -6784,7 +6784,7 @@
         </is>
       </c>
       <c r="D357">
-        <v>391.9509306202149</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="358">
@@ -6820,7 +6820,7 @@
         </is>
       </c>
       <c r="D359">
-        <v>103.6218025752549</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="360">
@@ -6838,7 +6838,7 @@
         </is>
       </c>
       <c r="D360">
-        <v>391.950930620215</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="361">
@@ -6856,7 +6856,7 @@
         </is>
       </c>
       <c r="D361">
-        <v>485.6083947034062</v>
+        <v>539.1303929564189</v>
       </c>
     </row>
     <row r="362">
@@ -6892,7 +6892,7 @@
         </is>
       </c>
       <c r="D363">
-        <v>103.6218025752549</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="364">
@@ -6910,7 +6910,7 @@
         </is>
       </c>
       <c r="D364">
-        <v>202.1265485002849</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="365">
@@ -6964,7 +6964,7 @@
         </is>
       </c>
       <c r="D367">
-        <v>202.1265485002849</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="368">
@@ -6982,7 +6982,7 @@
         </is>
       </c>
       <c r="D368">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="369">
@@ -7000,7 +7000,7 @@
         </is>
       </c>
       <c r="D369">
-        <v>202.1265485002849</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="370">
@@ -7054,7 +7054,7 @@
         </is>
       </c>
       <c r="D372">
-        <v>202.1265485002848</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="373">
@@ -7072,7 +7072,7 @@
         </is>
       </c>
       <c r="D373">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="374">
@@ -7108,7 +7108,7 @@
         </is>
       </c>
       <c r="D375">
-        <v>580.0967871035208</v>
+        <v>599.4029459436151</v>
       </c>
     </row>
     <row r="376">
@@ -7126,7 +7126,7 @@
         </is>
       </c>
       <c r="D376">
-        <v>297.8083388514165</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="377">
@@ -7144,7 +7144,7 @@
         </is>
       </c>
       <c r="D377">
-        <v>202.1265485002849</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="378">
@@ -7162,7 +7162,7 @@
         </is>
       </c>
       <c r="D378">
-        <v>580.0967871035208</v>
+        <v>599.4029459436151</v>
       </c>
     </row>
     <row r="379">
@@ -7180,7 +7180,7 @@
         </is>
       </c>
       <c r="D379">
-        <v>297.8083388514166</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="380">
@@ -7216,7 +7216,7 @@
         </is>
       </c>
       <c r="D381">
-        <v>778.3279848830533</v>
+        <v>742.5848606869374</v>
       </c>
     </row>
     <row r="382">
@@ -7234,7 +7234,7 @@
         </is>
       </c>
       <c r="D382">
-        <v>297.8083388514168</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="383">
@@ -7252,7 +7252,7 @@
         </is>
       </c>
       <c r="D383">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="384">
@@ -7270,7 +7270,7 @@
         </is>
       </c>
       <c r="D384">
-        <v>391.9509306202149</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="385">
@@ -7288,7 +7288,7 @@
         </is>
       </c>
       <c r="D385">
-        <v>885.5095393821996</v>
+        <v>846.0391805322009</v>
       </c>
     </row>
     <row r="386">
@@ -7306,7 +7306,7 @@
         </is>
       </c>
       <c r="D386">
-        <v>202.1265485002847</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="387">
@@ -7324,7 +7324,7 @@
         </is>
       </c>
       <c r="D387">
-        <v>297.8083388514166</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="388">
@@ -7342,7 +7342,7 @@
         </is>
       </c>
       <c r="D388">
-        <v>202.1265485002849</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="389">
@@ -7360,7 +7360,7 @@
         </is>
       </c>
       <c r="D389">
-        <v>778.3279848830533</v>
+        <v>742.5848606869376</v>
       </c>
     </row>
     <row r="390">
@@ -7378,7 +7378,7 @@
         </is>
       </c>
       <c r="D390">
-        <v>297.8083388514167</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="391">
@@ -7414,7 +7414,7 @@
         </is>
       </c>
       <c r="D392">
-        <v>103.621802575255</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="393">
@@ -7432,7 +7432,7 @@
         </is>
       </c>
       <c r="D393">
-        <v>391.950930620215</v>
+        <v>479.5431151996878</v>
       </c>
     </row>
     <row r="394">
@@ -7450,7 +7450,7 @@
         </is>
       </c>
       <c r="D394">
-        <v>297.8083388514164</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="395">
@@ -7504,7 +7504,7 @@
         </is>
       </c>
       <c r="D397">
-        <v>202.1265485002847</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="398">
@@ -7522,7 +7522,7 @@
         </is>
       </c>
       <c r="D398">
-        <v>202.1265485002849</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="399">
@@ -7540,7 +7540,7 @@
         </is>
       </c>
       <c r="D399">
-        <v>677.0733158492222</v>
+        <v>665.0053611702178</v>
       </c>
     </row>
     <row r="400">
@@ -7558,7 +7558,7 @@
         </is>
       </c>
       <c r="D400">
-        <v>297.8083388514166</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="401">
@@ -7576,7 +7576,7 @@
         </is>
       </c>
       <c r="D401">
-        <v>391.9509306202149</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="402">
@@ -7594,7 +7594,7 @@
         </is>
       </c>
       <c r="D402">
-        <v>103.621802575255</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="403">
@@ -7612,7 +7612,7 @@
         </is>
       </c>
       <c r="D403">
-        <v>391.9509306202152</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="404">
@@ -7630,7 +7630,7 @@
         </is>
       </c>
       <c r="D404">
-        <v>677.0733158492224</v>
+        <v>665.0053611702177</v>
       </c>
     </row>
     <row r="405">
@@ -7648,7 +7648,7 @@
         </is>
       </c>
       <c r="D405">
-        <v>580.0967871035214</v>
+        <v>599.4029459436151</v>
       </c>
     </row>
     <row r="406">
@@ -7666,7 +7666,7 @@
         </is>
       </c>
       <c r="D406">
-        <v>885.5095393821985</v>
+        <v>846.0391805322012</v>
       </c>
     </row>
     <row r="407">
@@ -7684,7 +7684,7 @@
         </is>
       </c>
       <c r="D407">
-        <v>297.8083388514166</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="408">
@@ -7738,7 +7738,7 @@
         </is>
       </c>
       <c r="D410">
-        <v>297.8083388514165</v>
+        <v>415.8096624832563</v>
       </c>
     </row>
     <row r="411">
@@ -7756,7 +7756,7 @@
         </is>
       </c>
       <c r="D411">
-        <v>202.1265485002847</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="412">
@@ -7774,7 +7774,7 @@
         </is>
       </c>
       <c r="D412">
-        <v>391.950930620215</v>
+        <v>479.5431151996877</v>
       </c>
     </row>
     <row r="413">
@@ -7792,7 +7792,7 @@
         </is>
       </c>
       <c r="D413">
-        <v>391.9509306202152</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="414">
@@ -7810,7 +7810,7 @@
         </is>
       </c>
       <c r="D414">
-        <v>202.1265485002848</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="415">
@@ -7828,7 +7828,7 @@
         </is>
       </c>
       <c r="D415">
-        <v>297.8083388514164</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="416">
@@ -7846,7 +7846,7 @@
         </is>
       </c>
       <c r="D416">
-        <v>202.1265485002847</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="417">
@@ -7900,7 +7900,7 @@
         </is>
       </c>
       <c r="D419">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="420">
@@ -7918,7 +7918,7 @@
         </is>
       </c>
       <c r="D420">
-        <v>485.6083947034064</v>
+        <v>539.1303929564186</v>
       </c>
     </row>
     <row r="421">
@@ -7972,7 +7972,7 @@
         </is>
       </c>
       <c r="D423">
-        <v>580.0967871035207</v>
+        <v>599.4029459436152</v>
       </c>
     </row>
     <row r="424">
@@ -7990,7 +7990,7 @@
         </is>
       </c>
       <c r="D424">
-        <v>202.1265485002848</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="425">
@@ -8008,7 +8008,7 @@
         </is>
       </c>
       <c r="D425">
-        <v>202.1265485002847</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="426">
@@ -8026,7 +8026,7 @@
         </is>
       </c>
       <c r="D426">
-        <v>103.6218025752549</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="427">
@@ -8044,7 +8044,7 @@
         </is>
       </c>
       <c r="D427">
-        <v>103.621802575255</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="428">
@@ -8062,7 +8062,7 @@
         </is>
       </c>
       <c r="D428">
-        <v>297.8083388514165</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="429">
@@ -8080,7 +8080,7 @@
         </is>
       </c>
       <c r="D429">
-        <v>202.1265485002848</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="430">
@@ -8134,7 +8134,7 @@
         </is>
       </c>
       <c r="D432">
-        <v>202.1265485002849</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="433">
@@ -8170,7 +8170,7 @@
         </is>
       </c>
       <c r="D434">
-        <v>391.9509306202152</v>
+        <v>479.5431151996881</v>
       </c>
     </row>
     <row r="435">
@@ -8188,7 +8188,7 @@
         </is>
       </c>
       <c r="D435">
-        <v>202.1265485002849</v>
+        <v>340.1864117793779</v>
       </c>
     </row>
     <row r="436">
@@ -8206,7 +8206,7 @@
         </is>
       </c>
       <c r="D436">
-        <v>297.8083388514165</v>
+        <v>415.8096624832563</v>
       </c>
     </row>
     <row r="437">
@@ -8224,7 +8224,7 @@
         </is>
       </c>
       <c r="D437">
-        <v>297.8083388514166</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="438">
@@ -8242,7 +8242,7 @@
         </is>
       </c>
       <c r="D438">
-        <v>103.6218025752551</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="439">
@@ -8278,7 +8278,7 @@
         </is>
       </c>
       <c r="D440">
-        <v>103.6218025752551</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="441">
@@ -8314,7 +8314,7 @@
         </is>
       </c>
       <c r="D442">
-        <v>297.8083388514165</v>
+        <v>415.8096624832563</v>
       </c>
     </row>
     <row r="443">
@@ -8332,7 +8332,7 @@
         </is>
       </c>
       <c r="D443">
-        <v>202.1265485002848</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="444">
@@ -8368,7 +8368,7 @@
         </is>
       </c>
       <c r="D445">
-        <v>202.1265485002848</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="446">
@@ -8404,7 +8404,7 @@
         </is>
       </c>
       <c r="D447">
-        <v>391.9509306202151</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="448">
@@ -8422,7 +8422,7 @@
         </is>
       </c>
       <c r="D448">
-        <v>297.8083388514165</v>
+        <v>415.8096624832563</v>
       </c>
     </row>
     <row r="449">
@@ -8440,7 +8440,7 @@
         </is>
       </c>
       <c r="D449">
-        <v>202.1265485002849</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="450">
@@ -8476,7 +8476,7 @@
         </is>
       </c>
       <c r="D451">
-        <v>580.0967871035214</v>
+        <v>599.4029459436154</v>
       </c>
     </row>
     <row r="452">
@@ -8494,7 +8494,7 @@
         </is>
       </c>
       <c r="D452">
-        <v>778.3279848830535</v>
+        <v>742.5848606869376</v>
       </c>
     </row>
     <row r="453">
@@ -8512,7 +8512,7 @@
         </is>
       </c>
       <c r="D453">
-        <v>202.1265485002847</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="454">
@@ -8530,7 +8530,7 @@
         </is>
       </c>
       <c r="D454">
-        <v>202.1265485002849</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="455">
@@ -8548,7 +8548,7 @@
         </is>
       </c>
       <c r="D455">
-        <v>202.1265485002848</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="456">
@@ -8566,7 +8566,7 @@
         </is>
       </c>
       <c r="D456">
-        <v>485.6083947034064</v>
+        <v>539.1303929564189</v>
       </c>
     </row>
     <row r="457">
@@ -8584,7 +8584,7 @@
         </is>
       </c>
       <c r="D457">
-        <v>297.8083388514166</v>
+        <v>415.8096624832563</v>
       </c>
     </row>
     <row r="458">
@@ -8602,7 +8602,7 @@
         </is>
       </c>
       <c r="D458">
-        <v>103.621802575255</v>
+        <v>233.0626819566948</v>
       </c>
     </row>
     <row r="459">
@@ -8620,7 +8620,7 @@
         </is>
       </c>
       <c r="D459">
-        <v>202.1265485002847</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="460">
@@ -8638,7 +8638,7 @@
         </is>
       </c>
       <c r="D460">
-        <v>103.6218025752551</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="461">
@@ -8656,7 +8656,7 @@
         </is>
       </c>
       <c r="D461">
-        <v>778.3279848830533</v>
+        <v>742.5848606869378</v>
       </c>
     </row>
     <row r="462">
@@ -8692,7 +8692,7 @@
         </is>
       </c>
       <c r="D463">
-        <v>297.8083388514165</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="464">
@@ -8710,7 +8710,7 @@
         </is>
       </c>
       <c r="D464">
-        <v>297.8083388514167</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="465">
@@ -8728,7 +8728,7 @@
         </is>
       </c>
       <c r="D465">
-        <v>103.621802575255</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="466">
@@ -8746,7 +8746,7 @@
         </is>
       </c>
       <c r="D466">
-        <v>580.0967871035216</v>
+        <v>599.4029459436154</v>
       </c>
     </row>
     <row r="467">
@@ -8764,7 +8764,7 @@
         </is>
       </c>
       <c r="D467">
-        <v>202.1265485002848</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="468">
@@ -8782,7 +8782,7 @@
         </is>
       </c>
       <c r="D468">
-        <v>485.6083947034061</v>
+        <v>539.1303929564187</v>
       </c>
     </row>
     <row r="469">
@@ -8800,7 +8800,7 @@
         </is>
       </c>
       <c r="D469">
-        <v>297.8083388514166</v>
+        <v>415.8096624832563</v>
       </c>
     </row>
     <row r="470">
@@ -8818,7 +8818,7 @@
         </is>
       </c>
       <c r="D470">
-        <v>485.6083947034064</v>
+        <v>539.1303929564187</v>
       </c>
     </row>
     <row r="471">
@@ -8836,7 +8836,7 @@
         </is>
       </c>
       <c r="D471">
-        <v>677.0733158492226</v>
+        <v>665.0053611702178</v>
       </c>
     </row>
     <row r="472">
@@ -8854,7 +8854,7 @@
         </is>
       </c>
       <c r="D472">
-        <v>580.0967871035208</v>
+        <v>599.4029459436151</v>
       </c>
     </row>
     <row r="473">
@@ -8872,7 +8872,7 @@
         </is>
       </c>
       <c r="D473">
-        <v>103.6218025752549</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="474">
@@ -8890,7 +8890,7 @@
         </is>
       </c>
       <c r="D474">
-        <v>103.621802575255</v>
+        <v>233.0626819566948</v>
       </c>
     </row>
     <row r="475">
@@ -8944,7 +8944,7 @@
         </is>
       </c>
       <c r="D477">
-        <v>297.8083388514166</v>
+        <v>415.8096624832563</v>
       </c>
     </row>
     <row r="478">
@@ -8962,7 +8962,7 @@
         </is>
       </c>
       <c r="D478">
-        <v>202.1265485002847</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="479">
@@ -8998,7 +8998,7 @@
         </is>
       </c>
       <c r="D480">
-        <v>103.6218025752549</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="481">
@@ -9016,7 +9016,7 @@
         </is>
       </c>
       <c r="D481">
-        <v>485.6083947034062</v>
+        <v>539.1303929564189</v>
       </c>
     </row>
     <row r="482">
@@ -9052,7 +9052,7 @@
         </is>
       </c>
       <c r="D483">
-        <v>202.1265485002849</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
     <row r="484">
@@ -9070,7 +9070,7 @@
         </is>
       </c>
       <c r="D484">
-        <v>485.6083947034061</v>
+        <v>539.130392956419</v>
       </c>
     </row>
     <row r="485">
@@ -9088,7 +9088,7 @@
         </is>
       </c>
       <c r="D485">
-        <v>485.6083947034061</v>
+        <v>539.130392956419</v>
       </c>
     </row>
     <row r="486">
@@ -9106,7 +9106,7 @@
         </is>
       </c>
       <c r="D486">
-        <v>391.950930620215</v>
+        <v>479.5431151996878</v>
       </c>
     </row>
     <row r="487">
@@ -9124,7 +9124,7 @@
         </is>
       </c>
       <c r="D487">
-        <v>297.8083388514165</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="488">
@@ -9142,7 +9142,7 @@
         </is>
       </c>
       <c r="D488">
-        <v>103.621802575255</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="489">
@@ -9160,7 +9160,7 @@
         </is>
       </c>
       <c r="D489">
-        <v>103.6218025752548</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="490">
@@ -9178,7 +9178,7 @@
         </is>
       </c>
       <c r="D490">
-        <v>202.1265485002848</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="491">
@@ -9196,7 +9196,7 @@
         </is>
       </c>
       <c r="D491">
-        <v>297.8083388514164</v>
+        <v>415.8096624832564</v>
       </c>
     </row>
     <row r="492">
@@ -9214,7 +9214,7 @@
         </is>
       </c>
       <c r="D492">
-        <v>391.9509306202149</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="493">
@@ -9232,7 +9232,7 @@
         </is>
       </c>
       <c r="D493">
-        <v>391.9509306202149</v>
+        <v>479.5431151996879</v>
       </c>
     </row>
     <row r="494">
@@ -9250,7 +9250,7 @@
         </is>
       </c>
       <c r="D494">
-        <v>103.6218025752551</v>
+        <v>233.0626819566949</v>
       </c>
     </row>
     <row r="495">
@@ -9286,7 +9286,7 @@
         </is>
       </c>
       <c r="D496">
-        <v>580.0967871035208</v>
+        <v>599.4029459436151</v>
       </c>
     </row>
     <row r="497">
@@ -9304,7 +9304,7 @@
         </is>
       </c>
       <c r="D497">
-        <v>391.950930620215</v>
+        <v>479.543115199688</v>
       </c>
     </row>
     <row r="498">
@@ -9322,7 +9322,7 @@
         </is>
       </c>
       <c r="D498">
-        <v>580.0967871035208</v>
+        <v>599.4029459436151</v>
       </c>
     </row>
     <row r="499">
@@ -9340,7 +9340,7 @@
         </is>
       </c>
       <c r="D499">
-        <v>202.1265485002848</v>
+        <v>340.186411779378</v>
       </c>
     </row>
     <row r="500">
@@ -9376,7 +9376,7 @@
         </is>
       </c>
       <c r="D501">
-        <v>202.1265485002849</v>
+        <v>340.1864117793781</v>
       </c>
     </row>
   </sheetData>

</xml_diff>